<commit_message>
revisi - 9 color chart, filepond
</commit_message>
<xml_diff>
--- a/public/assets/file/data-perusahaan/Format.xlsx
+++ b/public/assets/file/data-perusahaan/Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bkk\public\assets\file\data-perusahaan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F142778-4A87-450C-B039-13A2356692D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D44762-D905-4F4F-9DD9-4CAC0BF825D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{69AE1B6C-3BC2-4219-9C37-E56CBF36922A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>nama_perusahaan</t>
   </si>
@@ -42,16 +42,10 @@
     <t>bidang_usaha</t>
   </si>
   <si>
-    <t>alamat</t>
-  </si>
-  <si>
     <t>no_telepon</t>
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>Alamat lengkap, Kecamatan, Kelurahan, Kota/Kabupaten, Provinsi</t>
   </si>
 </sst>
 </file>
@@ -403,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5488D600-2C73-423E-BB16-6EF764A27065}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +413,7 @@
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,14 +426,6 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>